<commit_message>
Level design. Designe Level2
</commit_message>
<xml_diff>
--- a/Data/EnemyConfig.xlsx
+++ b/Data/EnemyConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13760" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13440" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -715,7 +715,7 @@
       </c>
       <c r="E3" s="1">
         <f xml:space="preserve"> VLOOKUP(B3,Sheet2!$A$2:$C$5,3) * VLOOKUP(C3, Sheet3!$A$2:$B$4,2)</f>
-        <v>297.5</v>
+        <v>255</v>
       </c>
       <c r="F3" s="1">
         <f>VLOOKUP(B3, Sheet2!$A$2:$D$5,4) * VLOOKUP(C3, Sheet3!$A$1:$F$4,6)</f>
@@ -749,7 +749,7 @@
       </c>
       <c r="E4" s="1">
         <f xml:space="preserve"> VLOOKUP(B4,Sheet2!$A$2:$C$5,3) * VLOOKUP(C4, Sheet3!$A$2:$B$4,2)</f>
-        <v>805</v>
+        <v>724.5</v>
       </c>
       <c r="F4" s="1">
         <f>VLOOKUP(B4, Sheet2!$A$2:$D$5,4) * VLOOKUP(C4, Sheet3!$A$1:$F$4,6)</f>
@@ -783,7 +783,7 @@
       </c>
       <c r="E5" s="1">
         <f xml:space="preserve"> VLOOKUP(B5,Sheet2!$A$2:$C$5,3) * VLOOKUP(C5, Sheet3!$A$2:$B$4,2)</f>
-        <v>2268</v>
+        <v>1944</v>
       </c>
       <c r="F5" s="1">
         <f>VLOOKUP(B5, Sheet2!$A$2:$D$5,4) * VLOOKUP(C5, Sheet3!$A$1:$F$4,6)</f>
@@ -817,7 +817,7 @@
       </c>
       <c r="E6" s="1">
         <f xml:space="preserve"> VLOOKUP(B6,Sheet2!$A$2:$C$5,3) * VLOOKUP(C6, Sheet3!$A$2:$B$4,2)</f>
-        <v>892.5</v>
+        <v>765</v>
       </c>
       <c r="F6" s="1">
         <f>VLOOKUP(B6, Sheet2!$A$2:$D$5,4) * VLOOKUP(C6, Sheet3!$A$1:$F$4,6)</f>
@@ -851,7 +851,7 @@
       </c>
       <c r="E7" s="1">
         <f xml:space="preserve"> VLOOKUP(B7,Sheet2!$A$2:$C$5,3) * VLOOKUP(C7, Sheet3!$A$2:$B$4,2)</f>
-        <v>2415</v>
+        <v>2173.5</v>
       </c>
       <c r="F7" s="1">
         <f>VLOOKUP(B7, Sheet2!$A$2:$D$5,4) * VLOOKUP(C7, Sheet3!$A$1:$F$4,6)</f>
@@ -885,7 +885,7 @@
       </c>
       <c r="E8" s="1">
         <f xml:space="preserve"> VLOOKUP(B8,Sheet2!$A$2:$C$5,3) * VLOOKUP(C8, Sheet3!$A$2:$B$4,2)</f>
-        <v>6804</v>
+        <v>5832</v>
       </c>
       <c r="F8" s="1">
         <f>VLOOKUP(B8, Sheet2!$A$2:$D$5,4) * VLOOKUP(C8, Sheet3!$A$1:$F$4,6)</f>
@@ -919,7 +919,7 @@
       </c>
       <c r="E9" s="1">
         <f xml:space="preserve"> VLOOKUP(B9,Sheet2!$A$2:$C$5,3) * VLOOKUP(C9, Sheet3!$A$2:$B$4,2)</f>
-        <v>446.25</v>
+        <v>382.5</v>
       </c>
       <c r="F9" s="1">
         <f>VLOOKUP(B9, Sheet2!$A$2:$D$5,4) * VLOOKUP(C9, Sheet3!$A$1:$F$4,6)</f>
@@ -953,7 +953,7 @@
       </c>
       <c r="E10" s="1">
         <f xml:space="preserve"> VLOOKUP(B10,Sheet2!$A$2:$C$5,3) * VLOOKUP(C10, Sheet3!$A$2:$B$4,2)</f>
-        <v>1207.5</v>
+        <v>1086.75</v>
       </c>
       <c r="F10" s="1">
         <f>VLOOKUP(B10, Sheet2!$A$2:$D$5,4) * VLOOKUP(C10, Sheet3!$A$1:$F$4,6)</f>
@@ -987,7 +987,7 @@
       </c>
       <c r="E11" s="1">
         <f xml:space="preserve"> VLOOKUP(B11,Sheet2!$A$2:$C$5,3) * VLOOKUP(C11, Sheet3!$A$2:$B$4,2)</f>
-        <v>3402</v>
+        <v>2916</v>
       </c>
       <c r="F11" s="1">
         <f>VLOOKUP(B11, Sheet2!$A$2:$D$5,4) * VLOOKUP(C11, Sheet3!$A$1:$F$4,6)</f>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="E12" s="1">
         <f xml:space="preserve"> VLOOKUP(B12,Sheet2!$A$2:$C$5,3) * VLOOKUP(C12, Sheet3!$A$2:$B$4,2)</f>
-        <v>267.75</v>
+        <v>229.5</v>
       </c>
       <c r="F12" s="1">
         <f>VLOOKUP(B12, Sheet2!$A$2:$D$5,4) * VLOOKUP(C12, Sheet3!$A$1:$F$4,6)</f>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="E13" s="1">
         <f xml:space="preserve"> VLOOKUP(B13,Sheet2!$A$2:$C$5,3) * VLOOKUP(C13, Sheet3!$A$2:$B$4,2)</f>
-        <v>724.5</v>
+        <v>652.05000000000007</v>
       </c>
       <c r="F13" s="1">
         <f>VLOOKUP(B13, Sheet2!$A$2:$D$5,4) * VLOOKUP(C13, Sheet3!$A$1:$F$4,6)</f>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="E14" s="1">
         <f xml:space="preserve"> VLOOKUP(B14,Sheet2!$A$2:$C$5,3) * VLOOKUP(C14, Sheet3!$A$2:$B$4,2)</f>
-        <v>2041.2</v>
+        <v>1749.6000000000001</v>
       </c>
       <c r="F14" s="1">
         <f>VLOOKUP(B14, Sheet2!$A$2:$D$5,4) * VLOOKUP(C14, Sheet3!$A$1:$F$4,6)</f>
@@ -1314,7 +1314,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1362,10 +1362,10 @@
       </c>
       <c r="B2" s="1">
         <f>C2 * E2</f>
-        <v>297.5</v>
+        <v>255</v>
       </c>
       <c r="C2" s="1">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
         <v>3</v>
@@ -1398,10 +1398,10 @@
       </c>
       <c r="B3" s="1">
         <f t="shared" ref="B3:B4" si="0">C3 * E3</f>
-        <v>805</v>
+        <v>724.5</v>
       </c>
       <c r="C3" s="1">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="D3" s="1">
         <v>7</v>
@@ -1434,10 +1434,10 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" si="0"/>
-        <v>2268</v>
+        <v>1944</v>
       </c>
       <c r="C4" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1">
         <v>12</v>

</xml_diff>